<commit_message>
Added High Availability and Scalability section
</commit_message>
<xml_diff>
--- a/AWS_SOLUTION_ARCHITECT_ASSOCIATE_CHEAT_SHEET.xlsx
+++ b/AWS_SOLUTION_ARCHITECT_ASSOCIATE_CHEAT_SHEET.xlsx
@@ -8,21 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AWS solution architect associate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3451492-A5B3-4A8C-A801-7557BA3975D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BB217F-F16D-4979-8568-7F0EFF702727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Information" sheetId="3" r:id="rId1"/>
     <sheet name="IAM" sheetId="1" r:id="rId2"/>
     <sheet name="EC2 Instance" sheetId="4" r:id="rId3"/>
     <sheet name="EC2 Instance Storage" sheetId="9" r:id="rId4"/>
-    <sheet name="AMI" sheetId="10" r:id="rId5"/>
-    <sheet name="Private &amp; Public IP" sheetId="6" r:id="rId6"/>
-    <sheet name="Placement Group" sheetId="7" r:id="rId7"/>
-    <sheet name="Network Interface(NIC or ENI)" sheetId="8" r:id="rId8"/>
-    <sheet name="Security Groups" sheetId="5" r:id="rId9"/>
-    <sheet name="Notes" sheetId="2" r:id="rId10"/>
+    <sheet name="HA &amp; Scalability" sheetId="11" r:id="rId5"/>
+    <sheet name="Load Balancer" sheetId="12" r:id="rId6"/>
+    <sheet name="ASG(Auto Scaling Group)" sheetId="14" r:id="rId7"/>
+    <sheet name="SSL or TLS" sheetId="13" r:id="rId8"/>
+    <sheet name="AMI" sheetId="10" r:id="rId9"/>
+    <sheet name="Private &amp; Public IP" sheetId="6" r:id="rId10"/>
+    <sheet name="Placement Group" sheetId="7" r:id="rId11"/>
+    <sheet name="Network Interface(NIC or ENI)" sheetId="8" r:id="rId12"/>
+    <sheet name="Security Groups" sheetId="5" r:id="rId13"/>
+    <sheet name="Notes" sheetId="2" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="338">
   <si>
     <t>Infrastructure URL</t>
   </si>
@@ -830,6 +834,9 @@
     <t>Can get a discount of up to 90% compared to On-demand</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>Define max spot price and get the instance while current spot price &lt; max
       The hourly spot price varies based on offer and capacity
       If the current spot price &gt; your max price you can choose to stop or terminate your instance
@@ -2168,6 +2175,701 @@
   </si>
   <si>
     <t>Better I/O performance as compared to other Storage option</t>
+  </si>
+  <si>
+    <t>Scalability &amp; High Availability</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>High Availability</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Run instances for the same application across multi AZ
+         Auto Scaling Group multi AZ
+         Load Balancer multi AZ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Horizontal Scaling</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Increase number of instances (= scale out / in)
+          Auto Scaling Group
+          Load Balancer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vertical Scaling</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Increase instance size (= scale up / down)
+          From: t2.nano - 0.5G of RAM, 1 vCPU
+          To: u-12tb1.metal – 12.3 TB of RAM, 448 vCPUs</t>
+    </r>
+  </si>
+  <si>
+    <t>What is load balancing?</t>
+  </si>
+  <si>
+    <t>Load Balances are servers that forward traffic to multiple servers (e.g., EC2 instances) downstream</t>
+  </si>
+  <si>
+    <t>Expose a single point of access (DNS) to your application</t>
+  </si>
+  <si>
+    <t>Seamlessly handle failures of downstream instances</t>
+  </si>
+  <si>
+    <t>Do regular health checks to your instances</t>
+  </si>
+  <si>
+    <t>Provide SSL termination (HTTPS) for your websites</t>
+  </si>
+  <si>
+    <t>Enforce stickiness with cookies</t>
+  </si>
+  <si>
+    <t>High availability across zones</t>
+  </si>
+  <si>
+    <t>Separate public traffic from private traffic</t>
+  </si>
+  <si>
+    <t>Why use an Elastic Load Balancer?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">An Elastic Load Balancer is a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>managed load balancer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+       AWS guarantees that it will be working
+       AWS takes care of upgrades, maintenance, high availability
+       AWS provides only a few configuration knobs</t>
+    </r>
+  </si>
+  <si>
+    <t>It costs less to setup your own load balancer but it will be a lot more effort on your end</t>
+  </si>
+  <si>
+    <t>It is integrated with many AWS offerings / services
+         EC2, EC2 Auto Scaling Groups, Amazon ECS
+         AWS Certificate Manager (ACM), CloudWatch
+         Route 53, AWS WAF, AWS Global Accelerator</t>
+  </si>
+  <si>
+    <t>Health Checks</t>
+  </si>
+  <si>
+    <t>Health Checks are crucial for Load Balancers</t>
+  </si>
+  <si>
+    <t>They enable the load balancer to know if instances it forwards traffic to are available to reply to requests</t>
+  </si>
+  <si>
+    <t>The health check is done on a port and a route (/health is common)</t>
+  </si>
+  <si>
+    <t>If the response is not 200 (OK), then the instance is unhealthy</t>
+  </si>
+  <si>
+    <t>Some load balancers can be setup as internal (private) or external (public) ELBs</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Application Load Balancer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (v2 - new generation) – 2016 – ALB
+         HTTP, HTTPS, WebSocket</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gateway Load Balancer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – 2020 – GWLB
+         Operates at layer 3 (Network layer) – IP Protocol</t>
+    </r>
+  </si>
+  <si>
+    <t>Load Balancer Security Groups allow HTTPS / HTTP From anywhere</t>
+  </si>
+  <si>
+    <t>Application Security Group: Allow traffic only from Load Balancer</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Network Load Balancer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (v2 - new generation) – 2017
+         TCP, TLS (secure TCP), UDP</t>
+    </r>
+  </si>
+  <si>
+    <t>ALB - Application Load Balancer (v2)</t>
+  </si>
+  <si>
+    <t>Application load balancers is Layer 7 (HTTP)</t>
+  </si>
+  <si>
+    <t>Load balancing to multiple HTTP applications across machines(target groups)</t>
+  </si>
+  <si>
+    <t>Load balancing to multiple applications on the same machine(ex: containers)</t>
+  </si>
+  <si>
+    <t>Support for HTTP/2 and WebSocket</t>
+  </si>
+  <si>
+    <t>Support redirects (from HTTP to HTTPS for example)</t>
+  </si>
+  <si>
+    <t>Routing tables to different target groups:
+     Routing based on path in URL (example.com/users &amp; example.com/posts)
+     Routing based on hostname in URL (one.example.com &amp; other.example.com)
+     Routing based on Query String, Headers (example.com/users?id=123&amp;order=false)</t>
+  </si>
+  <si>
+    <t>ALB are a great fit for micro services &amp; container-based application (example: Docker &amp; Amazon ECS)</t>
+  </si>
+  <si>
+    <t>Has a port mapping feature to redirect to a dynamic port in ECS</t>
+  </si>
+  <si>
+    <t>Fixed hostname (XXX.region.elb.amazonaws.com)</t>
+  </si>
+  <si>
+    <t>The application servers don’t see the IP of the client directly
+        The true IP of the client is inserted in the header X-Forwarded-For
+        We can also get Port (X-Forwarded-Port) and proto (X-Forwarded-Proto)</t>
+  </si>
+  <si>
+    <t>Target Groups</t>
+  </si>
+  <si>
+    <t>EC2 instances (can be managed by an Auto Scaling Group) – HTTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECS tasks (managed by ECS itself) – HTTP </t>
+  </si>
+  <si>
+    <t>Lambda functions – HTTP request is translated into a JSON event</t>
+  </si>
+  <si>
+    <t>IP Addresses – must be private IPs</t>
+  </si>
+  <si>
+    <t>ALB can route to multiple target groups</t>
+  </si>
+  <si>
+    <t>Health checks are at the target group level</t>
+  </si>
+  <si>
+    <t>Network Load Balancer (v2)</t>
+  </si>
+  <si>
+    <t>Network load balancers (Layer 4) allow to:
+          Forward TCP &amp; UDP traffic to your instances
+          Handle millions of request per seconds
+          Less latency ~100 ms (vs 400 ms for ALB)</t>
+  </si>
+  <si>
+    <t>NLB has one static IP per AZ, and supports assigning Elastic IP(helpful for whitelisting specific IP)</t>
+  </si>
+  <si>
+    <t>NLB are used for extreme performance, TCP or UDP traffic</t>
+  </si>
+  <si>
+    <t>EC2 instances</t>
+  </si>
+  <si>
+    <t>Application Load Balancer</t>
+  </si>
+  <si>
+    <t>Health Checks support the TCP, HTTP and HTTPS Protocols</t>
+  </si>
+  <si>
+    <t>NLB routes traffic at the TCP/UDP level, which means it does not have the ability to interpret the content of the HTTP requests.</t>
+  </si>
+  <si>
+    <t>When accessing your EC2 instances through an NLB, you can use either HTTP or TCP in your web browser. 
+However, NLB does not provide any specific HTTP-based routing or content-aware load balancing.</t>
+  </si>
+  <si>
+    <t>If you use HTTP, NLB will simply forward the HTTP traffic to the backend EC2 instances without analyzing the HTTP request details.</t>
+  </si>
+  <si>
+    <t>NLB does not have security Group,It directly forward the request to target groups which has security group</t>
+  </si>
+  <si>
+    <t>ALB has it own security group</t>
+  </si>
+  <si>
+    <t>Gateway Load Balancer</t>
+  </si>
+  <si>
+    <t>Operates at Layer 3 (Network Layer) – IP Packets</t>
+  </si>
+  <si>
+    <t>Deploy, scale, and manage a fleet of 3rd party network virtual appliances in AWS
+    Example: Firewalls, Intrusion Detection and Prevention Systems, Deep Packet Inspection Systems, payload manipulation, …</t>
+  </si>
+  <si>
+    <t>Combines the following functions:
+    Transparent Network Gateway – single entry/exit for all traffic
+    Load Balancer – distributes traffic to your virtual appliances</t>
+  </si>
+  <si>
+    <t>Uses the GENEVE protocol on port 6081</t>
+  </si>
+  <si>
+    <t>Sticky Session (Session Affinity)</t>
+  </si>
+  <si>
+    <t>It is possible to implement stickiness so that the same client is always redirected to the same instance behind a load balancer</t>
+  </si>
+  <si>
+    <t>This works for Classic Load Balancer,Application Load Balancer, and Network Load Balancer</t>
+  </si>
+  <si>
+    <t>For both CLB &amp; ALB, the “cookie” used for stickiness has an expiration date you control</t>
+  </si>
+  <si>
+    <t>Use case: make sure the user doesn’t lose his session data</t>
+  </si>
+  <si>
+    <t>Enabling stickiness may bring imbalance to the load over the backend EC2 instances</t>
+  </si>
+  <si>
+    <t>Application-based Cookies
+             Custom cookie
+                      Generated by the target
+                      Can include any custom attributes required by the application
+                      Cookie name must be specified individually for each target group
+                      Don’t use AWSALB, AWSALBAPP, or AWSALBTG (reserved for use by the ELB)
+            Application cookie
+                     Generated by the load balancer
+                     Cookie name is AWSALBAPP</t>
+  </si>
+  <si>
+    <t>Duration-based Cookies
+         Cookie generated by the load balancer 
+         Cookie name is AWSALB for ALB, AWSELB for CLB</t>
+  </si>
+  <si>
+    <t>Cross-Zone Load Balancing</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>With Cross Zone Load Balancing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:each load balancer instance distributes evenly across all registered instances in all AZ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Without Cross Zone Load Balancing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Requests are distributed in the instances of the node of the Elastic Load Balancer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Network Load Balancer &amp; Gateway Load Balancer:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+      Disabled by default
+      You pay charges ($) for inter AZ data if enabled</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Application Load Balancer : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+      Enabled by default (can be disabled at the Target Group level)
+      No charges for inter AZ data</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Classic Load Balancer:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+      Disabled by default
+      No charges for inter AZ data if enabled</t>
+    </r>
+  </si>
+  <si>
+    <t>SSL/TLS - Basics</t>
+  </si>
+  <si>
+    <t>An SSL Certificate allows traffic between your clients and your load balancer to be encrypted in transit (in-flight encryption)</t>
+  </si>
+  <si>
+    <t>SSL refers to Secure Sockets Layer, used to encrypt connections</t>
+  </si>
+  <si>
+    <t>TLS refers to Transport Layer Security, which is a newer version</t>
+  </si>
+  <si>
+    <t>SSL certificates have an expiration date (you set) and must be renewed</t>
+  </si>
+  <si>
+    <t>SSL Certificate on Load Balancer</t>
+  </si>
+  <si>
+    <t>The load balancer uses an X.509 certificate (SSL/TLS server certificate)</t>
+  </si>
+  <si>
+    <t>You can manage certificates using ACM (AWS Certificate Manager)</t>
+  </si>
+  <si>
+    <t>You can create upload your own certificates alternatively</t>
+  </si>
+  <si>
+    <t>HTTPS listener:
+      You must specify a default certificate
+      You can add an optional list of certs to support multiple domains
+      Clients can use SNI (Server Name Indication) to specify the hostname they reach
+      Ability to specify a security policy to support older versions of SSL / TLS (legacy clients)</t>
+  </si>
+  <si>
+    <t>SSL – Server Name Indication (SNI)</t>
+  </si>
+  <si>
+    <t>SNI solves the problem of loading multiple SSL certificates onto one web server (to serve multiple websites)</t>
+  </si>
+  <si>
+    <t>It’s a “newer” protocol, and requires the client to indicate the hostname of the target server in the initial SSL handshake</t>
+  </si>
+  <si>
+    <t>The server will then find the correct certificate, or return the default one</t>
+  </si>
+  <si>
+    <t>Only works for ALB &amp; NLB (newer generation), CloudFront</t>
+  </si>
+  <si>
+    <t>Does not work for CLB (older gen)</t>
+  </si>
+  <si>
+    <t>Supports multiple listeners with multiple SSL certificates,Uses Server Name Indication (SNI) to make it work</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Classic Load Balancer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (v1 - old generation) – 2009 – CLB : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Deprecated Not used now</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+         HTTP, HTTPS, TCP, SSL (secure TCP)
+         Support only one SSL certificate,Must use multiple CLB for multiple hostname with multiple SSL certificates</t>
+    </r>
+  </si>
+  <si>
+    <t>Connection Draining</t>
+  </si>
+  <si>
+    <t>Feature naming:
+     Connection Draining – for CLB
+     Deregistration Delay – for ALB &amp; NLB</t>
+  </si>
+  <si>
+    <t>Time to complete “in-flight requests” while the instance is de-registering or unhealthy</t>
+  </si>
+  <si>
+    <t>Stops sending new requests to the EC2 instance which is de-registering</t>
+  </si>
+  <si>
+    <t>Between 1 to 3600 seconds (default: 300 seconds)</t>
+  </si>
+  <si>
+    <t>Can be disabled (set value to 0)</t>
+  </si>
+  <si>
+    <t>Set to a low value if your requests are short</t>
+  </si>
+  <si>
+    <t>What’s an Auto Scaling Group</t>
+  </si>
+  <si>
+    <t>In real-life, the load on your websites and application can change</t>
+  </si>
+  <si>
+    <t>In the cloud, you can create and get rid of servers very quickly</t>
+  </si>
+  <si>
+    <t>The goal of an Auto Scaling Group (ASG) is to:
+       Scale out (add EC2 instances) to match an increased load
+       Scale in (remove EC2 instances) to match a decreased load
+       Ensure we have a minimum and a maximum number of EC2 instances running
+       Automatically register new instances to a load balancer
+       Re-create an EC2 instance in case a previous one is terminated (ex: if unhealthy)</t>
+  </si>
+  <si>
+    <t>ASG are free (you only pay for the underlying EC2 instances)</t>
+  </si>
+  <si>
+    <t>How New Automatic Instance get Created</t>
+  </si>
+  <si>
+    <t>Min Size / Max Size / Initial Capacity</t>
+  </si>
+  <si>
+    <t>A Launch Template (older “Launch Configurations” are deprecated) Used to create instances
+      AMI + Instance Type
+      EC2 User Data
+      EBS Volumes
+      Security Groups
+      SSH Key Pair
+      IAM Roles for your EC2 Instances
+      Network + Subnets Information
+      Load Balancer Information</t>
+  </si>
+  <si>
+    <t>Auto Scaling - CloudWatch Alarms &amp; Scaling</t>
+  </si>
+  <si>
+    <t>It is possible to scale an ASG based on CloudWatch alarms</t>
+  </si>
+  <si>
+    <t>An alarm monitors a metric (such as Average CPU, or a custom metric)</t>
+  </si>
+  <si>
+    <t>Metrics such as Average CPU are computed for the overall ASG instances</t>
+  </si>
+  <si>
+    <t>Based on the alarm:
+       We can create scale-out policies (increase the number of instances)
+       We can create scale-in policies (decrease the number of instances)</t>
   </si>
 </sst>
 </file>
@@ -2373,7 +3075,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2472,6 +3174,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3186,6 +3891,341 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7548946E-0D50-49AB-B4D1-E890484B2D04}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="90.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="17">
+        <v>1</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="B2" s="33" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" s="23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" s="23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" s="23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="17">
+        <v>2</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="B10" s="33" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="17">
+        <v>3</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" s="33" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" s="33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="2"/>
+      <c r="B18" s="42" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B19" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B20" s="33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B21" s="33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="32" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D074511F-8E9E-4D0F-8C8D-ABC1EBBE8007}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="91.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="17">
+        <v>1</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B2" s="23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" s="23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="290.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="32" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C005A05-B33E-4519-8153-1D35A073C306}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="70.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="17">
+        <v>1</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="B2" s="33" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="24" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="17">
+        <v>2</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" s="23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+      <c r="B8" s="33" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B9" s="33" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="24" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF6EBDCB-4DE0-49A1-A75F-AD165E6B90C3}">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="110" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="20">
+        <v>1</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B2" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" s="23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" s="23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B7" s="33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="101" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="23"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" s="23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" s="23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B14" s="33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" s="23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" s="42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="131" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="32" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1444A312-FFC7-465E-8080-F1CB10BBBB59}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -3444,7 +4484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9F54C5-C7E6-4CCD-AF80-7D8DC6717BA8}">
   <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView topLeftCell="B68" workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
@@ -3584,7 +4624,7 @@
     </row>
     <row r="33" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B33" s="33" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -3609,7 +4649,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B38" s="23" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -3639,22 +4679,22 @@
     </row>
     <row r="46" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="B46" s="33" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B47" s="33" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B48" s="33" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B49" s="33" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -3663,7 +4703,7 @@
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
       <c r="B51" s="40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="212" customHeight="1" x14ac:dyDescent="0.35">
@@ -3674,22 +4714,22 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B54" s="42" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B55" s="23" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="145" x14ac:dyDescent="0.35">
       <c r="B56" s="33" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B57" s="24" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -3698,22 +4738,22 @@
         <v>6</v>
       </c>
       <c r="B60" s="22" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B61" s="33" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B62" s="33" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B63" s="24" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -3722,37 +4762,37 @@
         <v>7</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B67" s="33" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="B68" s="33" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B69" s="33" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B70" s="33" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B71" s="33" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B72" s="32" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -3761,27 +4801,27 @@
         <v>8</v>
       </c>
       <c r="B75" s="36" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B76" s="23" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B77" s="23" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B78" s="23" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B79" s="24" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3795,7 +4835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7CCC42-89AA-44C3-988B-A74B99D58E9B}">
   <dimension ref="A1:B89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -3809,62 +4849,62 @@
         <v>1</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B2" s="42" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B3" s="33" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="23" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="23" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="23" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="23" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" s="33" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B9" s="23" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" s="23" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" s="23" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B12" s="33" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -3872,42 +4912,42 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B14" s="40" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B15" s="33" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B16" s="33" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" s="33" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" s="33" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" s="33" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" s="33" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" s="33" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.35">
@@ -3915,57 +4955,57 @@
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B23" s="40" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B24" s="23" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B25" s="23" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B26" s="23" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B27" s="23" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B28" s="23" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B29" s="23" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B30" s="23" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B31" s="23" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B32" s="23" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="24" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -3980,37 +5020,37 @@
         <v>2</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B39" s="23" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B40" s="23" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B41" s="33" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B42" s="33" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B43" s="33" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B44" s="32" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -4019,42 +5059,42 @@
         <v>3</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B48" s="23" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
       <c r="B49" s="33" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="174" x14ac:dyDescent="0.35">
       <c r="B50" s="33" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="B51" s="33" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="B52" s="33" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B53" s="23" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B54" s="23" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="318" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -4066,32 +5106,32 @@
         <v>4</v>
       </c>
       <c r="B58" s="22" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B59" s="23" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B60" s="33" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B61" s="33" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B62" s="42" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B63" s="24" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -4100,37 +5140,37 @@
         <v>5</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B67" s="33" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B68" s="23" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B69" s="23" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B70" s="23" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B71" s="23" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B72" s="23" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
@@ -4138,27 +5178,27 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B74" s="42" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B75" s="23" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B76" s="23" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B77" s="23" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B78" s="24" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -4167,22 +5207,22 @@
         <v>6</v>
       </c>
       <c r="B81" s="22" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B82" s="33" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B83" s="33" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="102" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B84" s="43" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -4191,17 +5231,17 @@
         <v>7</v>
       </c>
       <c r="B87" s="22" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B88" s="33" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B89" s="32" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -4211,6 +5251,754 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DECFAD2-42C6-491B-91E1-2BB880831D61}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="84" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="17">
+        <v>1</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="33" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B3" s="33" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="32" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="7" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="17">
+        <v>2</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" s="23" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" s="23" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" s="23" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" s="23" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" s="23" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B14" s="23" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="24" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B50A56A-D727-4F7B-877A-F95F5D50C0C4}">
+  <dimension ref="A1:B98"/>
+  <sheetViews>
+    <sheetView topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="105.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="17">
+        <v>1</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="B2" s="33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" s="33" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="B4" s="33" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" s="33"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" s="42" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" s="33" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="33" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" s="33" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="32" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="17">
+        <v>2</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B14" s="33" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B15" s="33" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B16" s="33" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B17" s="33" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="33" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B19" s="33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="35" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="17">
+        <v>3</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B24" s="23" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B25" s="23" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B26" s="23" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B27" s="23" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B28" s="23" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="B29" s="33" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B30" s="23" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B31" s="23" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B32" s="23" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B33" s="33" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B34" s="33" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B35" s="33" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B36" s="23"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B37" s="42" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B38" s="23" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B39" s="23" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B40" s="23" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B41" s="23" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B42" s="23" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B43" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="46" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="17">
+        <v>4</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="B47" s="33" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B48" s="23" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B49" s="23" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B50" s="23" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B51" s="33" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B52" s="33" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B53" s="33" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B54" s="33" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B55" s="33"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B56" s="42" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B57" s="23" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B58" s="23" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B59" s="23" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B60" s="24" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="63" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A63" s="17">
+        <v>5</v>
+      </c>
+      <c r="B63" s="22" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B64" s="33" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B65" s="23" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B66" s="33" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B67" s="23" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B68" s="23"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B69" s="42" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B70" s="23" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B71" s="24" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="74" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="17">
+        <v>6</v>
+      </c>
+      <c r="B74" s="22" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B75" s="23" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B76" s="23" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B77" s="23" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B78" s="23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B79" s="23" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="B80" s="33" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B81" s="32" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="84" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A84" s="17">
+        <v>7</v>
+      </c>
+      <c r="B84" s="22" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B85" s="23" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B86" s="23" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B87" s="33" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B88" s="33" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B89" s="32" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="92" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A92" s="17">
+        <v>8</v>
+      </c>
+      <c r="B92" s="36" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B93" s="33" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B94" s="23" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B95" s="23" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B96" s="23" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B97" s="23" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B98" s="24" t="s">
+        <v>324</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21A6A74-B165-49B1-9B17-2CC5EEE2A4BD}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="86.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="20">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+      <c r="B4" s="18" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" s="45" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="18" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="18" t="s">
+        <v>337</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A3E931-BAAF-4FAD-852F-C199231CE5D0}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="105.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="17">
+        <v>1</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B2" s="23" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" s="23" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" s="23" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" s="23" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" s="23"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" s="42" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" s="23" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" s="23" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" s="23" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="32" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="17">
+        <v>2</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" s="23" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" s="23" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="23" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="23" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="24" t="s">
+        <v>315</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C231497-3272-4EC9-A80A-1F1BA9FDD58E}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -4228,360 +6016,25 @@
         <v>1</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B2" s="18" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="B3" s="18" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="B4" s="18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7548946E-0D50-49AB-B4D1-E890484B2D04}">
-  <dimension ref="A1:B22"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="90.08984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="17">
-        <v>1</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="B2" s="33" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B3" s="23" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B4" s="23" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B5" s="23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="24" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="17">
-        <v>2</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="B10" s="33" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="32" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="17">
-        <v>3</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B15" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B16" s="33" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B17" s="23" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-      <c r="B18" s="42" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B19" s="23" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="B20" s="33" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B21" s="33" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="32" t="s">
-        <v>117</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D074511F-8E9E-4D0F-8C8D-ABC1EBBE8007}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="91.90625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="17">
-        <v>1</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B3" s="23" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="290.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C005A05-B33E-4519-8153-1D35A073C306}">
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="70.26953125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="17">
-        <v>1</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="B2" s="33" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="24" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="17">
-        <v>2</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B7" s="23" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="B8" s="33" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="B9" s="33" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="24" t="s">
-        <v>134</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF6EBDCB-4DE0-49A1-A75F-AD165E6B90C3}">
-  <dimension ref="A1:B18"/>
-  <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="110" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="20">
-        <v>1</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B3" s="23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B4" s="23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B5" s="23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B6" s="23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B7" s="33" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="101" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="23"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B9" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B10" s="23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B11" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B12" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B13" s="23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="B14" s="33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B15" s="23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B16" s="42" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" ht="131" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="32" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B18" s="21"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>